<commit_message>
fixed figure 2 linetype error
</commit_message>
<xml_diff>
--- a/Outcome/fig data/fig 2.xlsx
+++ b/Outcome/fig data/fig 2.xlsx
@@ -430,7 +430,7 @@
         <v>94.751368232637</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="3">
@@ -450,7 +450,7 @@
         <v>83.1428673394735</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         <v>49.7553235705404</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         <v>50.365843943148</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +510,7 @@
         <v>47.4224844491716</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="7">
@@ -530,7 +530,7 @@
         <v>13.4670557036886</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="8">
@@ -550,7 +550,7 @@
         <v>2.1218244341509</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="9">
@@ -570,7 +570,7 @@
         <v>1.84128198914687</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="10">
@@ -590,7 +590,7 @@
         <v>9.23631643219175</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="11">
@@ -610,7 +610,7 @@
         <v>0.489267734481886</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="12">
@@ -630,7 +630,7 @@
         <v>0.405381399053675</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="13">
@@ -650,7 +650,7 @@
         <v>0.747513275782065</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="14">
@@ -670,7 +670,7 @@
         <v>1.5853845206178</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="15">
@@ -690,7 +690,7 @@
         <v>2.16103645145237</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="16">
@@ -710,7 +710,7 @@
         <v>0.351245378315242</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="17">
@@ -730,7 +730,7 @@
         <v>0.642544497755498</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="18">
@@ -750,7 +750,7 @@
         <v>2.78991186524577</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="19">
@@ -770,7 +770,7 @@
         <v>2.67979011757543</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="20">
@@ -790,7 +790,7 @@
         <v>4.62403895574973</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="21">
@@ -810,7 +810,7 @@
         <v>6.78240230252582</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         <v>4.94060343431426</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="23">
@@ -850,7 +850,7 @@
         <v>3.90468630621018</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="24">
@@ -870,7 +870,7 @@
         <v>5.94800803052963</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="25">
@@ -890,7 +890,7 @@
         <v>2.08024297953784</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="26">
@@ -910,7 +910,7 @@
         <v>0.746124025030856</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="27">
@@ -930,7 +930,7 @@
         <v>0.663615855711427</v>
       </c>
       <c r="F27" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="28">
@@ -950,7 +950,7 @@
         <v>2.577623903768</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="29">
@@ -970,7 +970,7 @@
         <v>2.10135983835969</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="30">
@@ -990,7 +990,7 @@
         <v>2.32373443731324</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="31">
@@ -1010,7 +1010,7 @@
         <v>1.30583271736557</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="32">
@@ -1030,7 +1030,7 @@
         <v>6.27614403278498</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="33">
@@ -1050,7 +1050,7 @@
         <v>9.4068227161278</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="34">
@@ -1070,7 +1070,7 @@
         <v>1.62881065192344</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="35">
@@ -1090,7 +1090,7 @@
         <v>0.451800471221472</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="36">
@@ -1110,7 +1110,7 @@
         <v>0.283174835564165</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="37">
@@ -1130,7 +1130,7 @@
         <v>0.661018872753891</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="38">
@@ -1150,7 +1150,7 @@
         <v>27.3821012113911</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="39">
@@ -1170,7 +1170,7 @@
         <v>24.5282804647134</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="40">
@@ -1190,7 +1190,7 @@
         <v>46.8369617581369</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="41">
@@ -1210,7 +1210,7 @@
         <v>62.2916979261866</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="42">
@@ -1230,7 +1230,7 @@
         <v>25.5694959945828</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="43">
@@ -1250,7 +1250,7 @@
         <v>3.71458290914476</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="44">
@@ -1270,7 +1270,7 @@
         <v>1.20864119975184</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="45">
@@ -1290,7 +1290,7 @@
         <v>0.347135940459244</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="46">
@@ -1310,7 +1310,7 @@
         <v>2.69696473833369</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="47">
@@ -1330,7 +1330,7 @@
         <v>6.13238530446963</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="48">
@@ -1350,7 +1350,7 @@
         <v>6.82184642566895</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="49">
@@ -1370,7 +1370,7 @@
         <v>8.00342805216446</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="50">
@@ -1390,7 +1390,7 @@
         <v>7.2719772634103</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="51">
@@ -1410,7 +1410,7 @@
         <v>7.61595226453572</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="52">
@@ -1430,7 +1430,7 @@
         <v>2.59427901682998</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="53">
@@ -1450,7 +1450,7 @@
         <v>0.105091220612554</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="54">
@@ -1470,7 +1470,7 @@
         <v>0.123230376249829</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="55">
@@ -1490,7 +1490,7 @@
         <v>1.29098086841739</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="56">
@@ -1510,7 +1510,7 @@
         <v>1.00884634349837</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="57">
@@ -1530,7 +1530,7 @@
         <v>1.36556223611166</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="58">
@@ -1550,7 +1550,7 @@
         <v>1.3704601988</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="59">
@@ -1570,7 +1570,7 @@
         <v>1.85741374226475</v>
       </c>
       <c r="F59" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="60">
@@ -1590,7 +1590,7 @@
         <v>1.05686532041344</v>
       </c>
       <c r="F60" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="61">
@@ -1610,7 +1610,7 @@
         <v>0.186129321468097</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="62">
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="63">
@@ -1650,7 +1650,7 @@
         <v>0.0334689467163491</v>
       </c>
       <c r="F63" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="64">
@@ -1670,7 +1670,7 @@
         <v>0.3325173910752</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="65">
@@ -1690,7 +1690,7 @@
         <v>2.37424995885766</v>
       </c>
       <c r="F65" s="1" t="n">
-        <v>42186</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="66">
@@ -1710,7 +1710,7 @@
         <v>1.86424507465993</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>42552</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="67">
@@ -1730,7 +1730,7 @@
         <v>1.76778502908069</v>
       </c>
       <c r="F67" s="1" t="n">
-        <v>42917</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="68">
@@ -1750,7 +1750,7 @@
         <v>1.20250483201683</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>43282</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="69">
@@ -1770,7 +1770,7 @@
         <v>1.4492117657193</v>
       </c>
       <c r="F69" s="1" t="n">
-        <v>43647</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="70">
@@ -1790,7 +1790,7 @@
         <v>0.560811086548158</v>
       </c>
       <c r="F70" s="1" t="n">
-        <v>44013</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="71">
@@ -1810,7 +1810,7 @@
         <v>0.153116806544606</v>
       </c>
       <c r="F71" s="1" t="n">
-        <v>44378</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="72">
@@ -1830,7 +1830,7 @@
         <v>0.254811068722052</v>
       </c>
       <c r="F72" s="1" t="n">
-        <v>44743</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="73">
@@ -1850,7 +1850,7 @@
         <v>0.738830997037416</v>
       </c>
       <c r="F73" s="1" t="n">
-        <v>45108</v>
+        <v>44927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>